<commit_message>
Updated pin spreadsheet (moved PWM)
</commit_message>
<xml_diff>
--- a/Trenz_GPIO_pins (1).xlsx
+++ b/Trenz_GPIO_pins (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhass\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C13AC2-0DD5-4394-9348-5EFA9B63C3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE130FA-B6C4-4BD3-9D2B-AE3B03F88A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
   <si>
     <t>5V</t>
   </si>
@@ -252,6 +252,18 @@
   </si>
   <si>
     <t>clk_gen</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>white</t>
   </si>
 </sst>
 </file>
@@ -893,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K25"/>
+  <dimension ref="B2:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="92" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -906,11 +918,12 @@
     <col min="4" max="7" width="9.1328125" style="1"/>
     <col min="8" max="8" width="18.40625" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.26953125" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" style="1"/>
+    <col min="11" max="12" width="8.7265625" style="1"/>
+    <col min="13" max="13" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
-    <row r="3" spans="2:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="2" spans="2:12" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
+    <row r="3" spans="2:12" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="C3" s="29" t="s">
         <v>2</v>
       </c>
@@ -920,15 +933,18 @@
       <c r="G3" s="30"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="2:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="4" spans="2:12" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="J4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.75">
+      <c r="L4" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.75">
       <c r="C5" s="19"/>
       <c r="D5" s="20" t="s">
         <v>3</v>
@@ -950,7 +966,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.75">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.75">
       <c r="B6" t="s">
         <v>70</v>
       </c>
@@ -979,7 +995,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.75">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.75">
       <c r="B7" t="s">
         <v>70</v>
       </c>
@@ -1008,7 +1024,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.75">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.75">
       <c r="C8" s="23" t="s">
         <v>13</v>
       </c>
@@ -1034,7 +1050,7 @@
       </c>
       <c r="K8" s="28"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.75">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.75">
       <c r="C9" s="23"/>
       <c r="D9" s="4" t="s">
         <v>1</v>
@@ -1058,7 +1074,7 @@
       </c>
       <c r="K9" s="28"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.75">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.75">
       <c r="C10" s="11" t="s">
         <v>47</v>
       </c>
@@ -1085,7 +1101,7 @@
       </c>
       <c r="K10" s="28"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.75">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.75">
       <c r="C11" s="23" t="s">
         <v>57</v>
       </c>
@@ -1111,7 +1127,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.75">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.75">
       <c r="C12" s="23" t="s">
         <v>52</v>
       </c>
@@ -1139,7 +1155,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.75">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.75">
       <c r="C13" s="23"/>
       <c r="D13" s="2" t="s">
         <v>3</v>
@@ -1165,7 +1181,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.75">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.75">
       <c r="C14" s="23" t="s">
         <v>40</v>
       </c>
@@ -1191,7 +1207,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.75">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.75">
       <c r="C15" s="23" t="s">
         <v>19</v>
       </c>
@@ -1215,11 +1231,8 @@
       <c r="J15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.75">
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.75">
       <c r="C16" s="23" t="s">
         <v>41</v>
       </c>
@@ -1244,7 +1257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.75">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.75">
       <c r="C17" s="23"/>
       <c r="D17" s="4" t="s">
         <v>1</v>
@@ -1269,8 +1282,11 @@
       <c r="K17" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.75">
+      <c r="L17" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.75">
       <c r="C18" s="23"/>
       <c r="D18" s="3" t="s">
         <v>33</v>
@@ -1293,8 +1309,11 @@
       <c r="K18" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.75">
+      <c r="L18" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.75">
       <c r="C19" s="23" t="s">
         <v>14</v>
       </c>
@@ -1317,7 +1336,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.75">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.75">
       <c r="C20" s="23" t="s">
         <v>15</v>
       </c>
@@ -1342,7 +1361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.75">
+    <row r="21" spans="3:13" x14ac:dyDescent="0.75">
       <c r="C21" s="11" t="s">
         <v>43</v>
       </c>
@@ -1365,7 +1384,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.75">
+    <row r="22" spans="3:13" x14ac:dyDescent="0.75">
       <c r="C22" s="11" t="s">
         <v>49</v>
       </c>
@@ -1389,8 +1408,15 @@
       <c r="J22" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.75">
+      <c r="K22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.75">
       <c r="C23" s="11" t="s">
         <v>56</v>
       </c>
@@ -1415,7 +1441,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="3:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="24" spans="3:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="C24" s="25"/>
       <c r="D24" s="26" t="s">
         <v>1</v>
@@ -1440,13 +1466,19 @@
       <c r="K24" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="25" spans="3:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="L24" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="J25" s="27" t="s">
         <v>39</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>69</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>